<commit_message>
updated the write group and write material
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>material vendor code</t>
   </si>
@@ -30,6 +30,12 @@
   </si>
   <si>
     <t>group name</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Майки / Футболки / Рубашки / Комбинезоны</t>
   </si>
 </sst>
 </file>
@@ -104,8 +110,11 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>6</v>
+      </c>
       <c r="D3" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>